<commit_message>
Update Chinese and PTBR language files to 23.260
Added and updated multiple Chinese language .xlsx and .txt files for game data, dialogs, and text resources to version 23.260. Also added corresponding PTBR update log. Changes include new and revised entries for character talk, god talk, dialog, game objects, and other language assets.
</commit_message>
<xml_diff>
--- a/new original/_Lang_Chinese/Lang/CN/Dialog/dialog.xlsx
+++ b/new original/_Lang_Chinese/Lang/CN/Dialog/dialog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="647">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -2378,203 +2378,386 @@
 That witch’s bakery in Mysilia is so lovely... A real shop, right in the city. A witch... and a baker!</t>
   </si>
   <si>
+    <t xml:space="preserve">rodwyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">私の料理に使われているのは全部最高級の素材。
+私のホウキコレクション、見てみたい？
+ええと…イモリの舌に…ハチの目。あら？ ごめんなさい、そこにいるのに気づかなかったわ。新しいレシピを考えていたの。
+あれ、この辺りにネコいなかった？
+もちろんパンは窯で焼けるわよ？ 
+薬棚？  ちゃんと見なさい、スパイスの棚でしょ！
+私の帽子？　ふふ、素敵でしょ？
+（魔女は虫が詰まっているような袋をミキシングボウルにどさっと入れた。）
+……質問が多いのねぇ…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I only use the highest quality ingredients for my baked goods.
+Would you like to see my broom collection?
+Let’s see…Tongue of newt. Eye of bee. Oh? Sorry, I didn’t notice you there. I was thinking of a new recipe.
+Have you seen any cats nearby?
+Of course you can bake bread in a kiln! Don’t you?
+My chemistry rack? Those are obviously spices!
+My hat? Cool right?
+(You watch her dump what appears to be a sack of bugs into a mixing bowl.) 
+You sure do ask a lot of questions…</t>
+  </si>
+  <si>
     <t xml:space="preserve">eyth</t>
   </si>
   <si>
-    <t xml:space="preserve">@2…ピー…
-@2…ザザザ…
-@2…ザザ…ガガ…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…bneep…
-@2…zzzzzz…
-@2…zshh…beep……</t>
+    <t xml:space="preserve">…ピー…
+…ザザザ…
+…ザザ…ガガ…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…bneep…
+…zzzzzz…
+…zshh…beep……</t>
   </si>
   <si>
     <t xml:space="preserve">jure</t>
   </si>
   <si>
-    <t xml:space="preserve">@2…なで…なで…
-@2…ぎゅぅーっ…
-@2…ぎゅーーーーっ…
-@2…よし…よし…
-@2…ば…ばか…
-@2…か…勘違いしないでよね…
-@2…べ…べつに…あなたのためじゃ…
-@2…べ…べつに…
-@2…ひ…暇だっただけなんだからね…
-@2…んっ…っしょ…
-@2…い…癒やされなさい…
-@2…ふ…ふあぁぁ…
-@2…えっほ…えっほ…
-@2…迷える…ものたちよ…
-@2…い…癒やし…
-@2…傷ついた…魂を…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…p-pat…pat…
-@2…huuug…
-@2…huuuuuug…
-@2…there you go…there you go…
-@2…y-you idiot…
-@2…d-don’t get the wrong idea, okay…
-@2…i-it’s not like i’m doing this for you or anything…
-@2…i-it’s…really not…
-@2…i just…h-happened to have some time, that’s all…
-@2…mm…there…
-@2…y-you should…let yourself relax…
-@2…f-fuuaaah…
-@2…eh-ho…eh-ho…
-@2…oh…you who wander…
-@2…h-healing…
-@2…for your…wounded souls…</t>
+    <t xml:space="preserve">…なで…なで…
+…ぎゅぅーっ…
+…ぎゅーーーーっ…
+…よし…よし…
+…ば…ばか…
+…か…勘違いしないでよね…
+…べ…べつに…あなたのためじゃ…
+…べ…べつに…
+…ひ…暇だっただけなんだからね…
+…んっ…っしょ…
+…い…癒やされなさい…
+…ふ…ふあぁぁ…
+…えっほ…えっほ…
+…迷える…ものたちよ…
+…い…癒やし…
+…傷ついた…魂を…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…p-pat…pat…
+…huuug…
+…huuuuuug…
+…there you go…there you go…
+…y-you idiot…
+…d-don’t get the wrong idea, okay…
+…i-it’s not like i’m doing this for you or anything…
+…i-it’s…really not…
+…i just…h-happened to have some time, that’s all…
+…mm…there…
+…y-you should…let yourself relax…
+…f-fuuaaah…
+…eh-ho…eh-ho…
+…oh…you who wander…
+…h-healing…
+…for your…wounded souls…</t>
   </si>
   <si>
     <t xml:space="preserve">opatos</t>
   </si>
   <si>
-    <t xml:space="preserve">@2…ゴリ…ゴリゴリ…
-@2…ゴゴゴゴ……
-@2…ズズズ……
-@2…ドシャァ……
-@2…ズシャッ…ズシャァ……
-@2…ガリ…ガリガリ……
-@2…ゴォ……ゴォォ……
-@2…ミシ…ミシミシ……
-@2…バキ……バキバキ……
-@2…ザラ……ザラザラ……
-@2…ゴン……ゴン……
-@2…ズン……ズゥン……
-@2…ドゥン……
-@2…フハハハハハハハ……
-@2…フハハ……フハァ……
-@2…フハーン……
-@2…フフ……フハ……
+    <t xml:space="preserve">…ゴリ…ゴリゴリ…
+…ゴゴゴゴ……
+…ズズズ……
+…ドシャァ……
+…ズシャッ…ズシャァ……
+…ガリ…ガリガリ……
+…ゴォ……ゴォォ……
+…ミシ…ミシミシ……
+…バキ……バキバキ……
+…ザラ……ザラザラ……
+…ゴン……ゴン……
+…ズン……ズゥン……
+…ドゥン……
+…フハハハハハハハ……
+…フハハ……フハァ……
+…フハーン……
+…フフ……フハ……
 @3フハハハハハハハハハハハハハ！ 
 @3フハーン
-@2…フフ……
-@2…フー…！…フー…！……</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…grrr…grind grind…
-@2…goooogoooo……
-@2…rumble……
-@2…crashhh……
-@2…shrrk…shraaa……
-@2…scrape…scrrrape……
-@2…gooo……grooo……
-@2…creak…craaack……
-@2…crack…crack crack……
-@2…grain…grind grind……
-@2…thud……thud……
-@2…boom……booom……
-@2…dunn……
-@2…muwahaha…
-@2…mwahahahaha…
-@2…muhan…
-@2…muwaha…muwaha…
+…フフ……
+…フー…！…フー…！……</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…grrr…grind grind…
+…goooogoooo……
+…rumble……
+…crashhh……
+…shrrk…shraaa……
+…scrape…scrrrape……
+…gooo……grooo……
+…creak…craaack……
+…crack…crack crack……
+…grain…grind grind……
+…thud……thud……
+…boom……booom……
+…dunn……
+…muwahaha…
+…mwahahahaha…
+…muhan…
+…muwaha…muwaha…
 @3MUWAHAHAHAHAHAHAHA!
 @3MUHAN
-@2…muha……
-@2…mu…ha……mu…ha……</t>
+…muha……
+…mu…ha……mu…ha……</t>
   </si>
   <si>
     <t xml:space="preserve">horome</t>
   </si>
   <si>
-    <t xml:space="preserve">@2…大丈夫…ママがちゃんとそばにいるからね…
-@2…おやすみ…いい子…
-@2…ママのお胸に…もたれてもいいよ…
-@2…ちゃんと生きてるだけで…えらい…
-@2…ほら…頭なでなで…安心して…
-@2…ほら…力を抜いて…
-@2…よしよし…
-@2…このまま…ぬくぬくしていきましょ…
-@2…なで…なで…力、抜いて…
-@2…ん…よしよし…いい子…
-@2…ぬくぬく…このまま…
-@2…もう…何も考えなくて…
-@2…ふわふわでしょう…落ち着くわね…
-@2…この尻尾…巻いてあげる…
-@2…ふわ…もふ…ほら…尻尾…
-@2…すり…すり…やさしく…巻くわね…
-@2…ぬく…ぬく…眠くなる…
-@2…そのまま…くっついて…
-@2…すぅ…はぁ…一緒に…呼吸…
-@2…ママだよ…
-@2…なで…なで…力…抜いて…
-@2…ほら…ぎゅううぅぅぅううっ…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…it’s okay…mommy’s right here with you…
-@2…good night…sweet one…
-@2…you can rest against mommy…it’s okay…
-@2…just being here…is already enough…
-@2…here…gentle head pats…you’re safe…
-@2…that’s it…relax…
-@2…there there…
-@2…let’s stay warm…just like this…
-@2…pat…pat…let it go…
-@2…mm…there there…good one…
-@2…warm…cozy…just like this…
-@2…no more thinking…now…
-@2…fluffy, isn’t it…it calms you…
-@2…i’ll wrap you…with my tail…
-@2…fluff…mofu…here…my tail…
-@2…rub…rub…gently…wrapping you…
-@2…warm…cozy…getting sleepy…
-@2…stay close…like that…
-@2…inhale…exhale…with me…
-@2…it’s mommy…
-@2…pat…pat…let it go…
-@2…there…huuuuuuuuuug…</t>
+    <t xml:space="preserve">…大丈夫…ママがちゃんとそばにいるからね…
+…おやすみ…いい子…
+…ママのお胸に…もたれてもいいよ…
+…ちゃんと生きてるだけで…えらい…
+…ほら…頭なでなで…安心して…
+…ほら…力を抜いて…
+…よしよし…
+…このまま…ぬくぬくしていきましょ…
+…なで…なで…力、抜いて…
+…ん…よしよし…いい子…
+…ぬくぬく…このまま…
+…もう…何も考えなくて…
+…ふわふわでしょう…落ち着くわね…
+…この尻尾…巻いてあげる…
+…ふわ…もふ…ほら…尻尾…
+…すり…すり…やさしく…巻くわね…
+…ぬく…ぬく…眠くなる…
+…そのまま…くっついて…
+…すぅ…はぁ…一緒に…呼吸…
+…ママだよ…
+…なで…なで…力…抜いて…
+…ほら…ぎゅううぅぅぅううっ…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…it’s okay…mommy’s right here with you…
+…good night…sweet one…
+…you can rest against mommy…it’s okay…
+…just being here…is already enough…
+…here…gentle head pats…you’re safe…
+…that’s it…relax…
+…there there…
+…let’s stay warm…just like this…
+…pat…pat…let it go…
+…mm…there there…good one…
+…warm…cozy…just like this…
+…no more thinking…now…
+…fluffy, isn’t it…it calms you…
+…i’ll wrap you…with my tail…
+…fluff…mofu…here…my tail…
+…rub…rub…gently…wrapping you…
+…warm…cozy…getting sleepy…
+…stay close…like that…
+…inhale…exhale…with me…
+…it’s mommy…
+…pat…pat…let it go…
+…there…huuuuuuuuuug…</t>
   </si>
   <si>
     <t xml:space="preserve">demitas</t>
   </si>
   <si>
-    <t xml:space="preserve">@2…ククク……
-@2…クク……
-@2…ク……ククク……
-@2…クク……クク…
-@2…ほら…還れ…
-@2…元素へ……
-@2…還れ…
-@2…元素へ…クク…
-@2…ク…ク…ク……
-@2…ク…ク…
-@2…クク…ク…
-@2…はやく…
-@2…クククク…
-@2…ククククク…
-@2…クク…クク…クク…
-@2………
-@2………
-@2……キウイ…クク…
-@2……
-@2…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…heh heh heh……
-@2…heh heh……
-@2…heh……heh heh……
-@2…heh heh……heh heh…
-@2…now… return…
-@2…to the elements……
-@2…return…
-@2…to the elements… heh heh…
-@2…heh… heh… heh……
-@2…heh… heh…
-@2…heh heh… heh…
-@2…hurry…
-@2…heh heh heh heh…
-@2…heh heh heh heh heh…
-@2…heh heh… heh heh… heh heh…
-@2………
-@2………
-@2……kiwi… heh heh…
-@2……
-@2… </t>
+    <t xml:space="preserve">…ククク……
+…クク……
+…ク……ククク……
+…クク……クク…
+…ほら…還れ…
+…元素へ……
+…還れ…
+…元素へ…クク…
+…ク…ク…ク……
+…ク…ク…
+…クク…ク…
+…はやく…
+…クククク…
+…ククククク…
+…クク…クク…クク…
+………
+………
+……キウイ…クク…
+……
+…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…heh heh heh……
+…heh heh……
+…heh……heh heh……
+…heh heh……heh heh…
+…now… return…
+…to the elements……
+…return…
+…to the elements… heh heh…
+…heh… heh… heh……
+…heh… heh…
+…heh heh… heh…
+…hurry…
+…heh heh heh heh…
+…heh heh heh heh heh…
+…heh heh… heh heh… heh heh…
+………
+………
+……kiwi… heh heh…
+……
+… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lulwy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…ふぅん…こういうのが好きなの…？
+…とんだ変態ね… 
+…この…豚野郎……アハハ……！
+…あら…震えてる……かわいそうに…
+…見下されるの…好きでしょう…？
+…虫ケラの分際で……アハハハ… 
+…小さい……ほんと……小さい……
+…アハ……笑えるわ……
+…アハハ……ミンチ……ミンチィ……！
+…哀れね……
+…ほら…もっと晒しなさい…
+…女神の前で…よくそんな顔できるわね…
+…アハハ…みじめな豚… 
+…その顔…最高に…無様ねぇ…
+…ほら…地面に這いつくばりなさい…
+…アハ…風も笑ってるわよ…
+…誰が…女神を見ていいって…言った…？
+…次に顔上げたら…ミンチよ…
+…アハッ…みじめな定命者ァ…
+…ほんと…分かりやすい…
+…アハハ…どうしようもないわね…
+…無様ね…罵られて…喜んじゃって…
+…この…変態…
+…ああ…今の…嬉しかったでしょ…？
+…ゴミが…
+…そのまま…無価値でいなさい…
+…ねえ…下心でもあるの…？
+…ああ…図星ね……アハハ！
+…存在してるだけで…不快…アハッ…
+…ほんと…救いようのない変態ね…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…oh… so this is what you like…?
+…what a degenerate…
+…you… filthy pig… ahaha…!
+…oh… you’re trembling… how adorable…
+…you like being looked down on… don’t you…?
+…a mere insect… ahahaha…
+…so small… truly… tiny…
+…aha… amusing…
+…ahaha… minced… so minced…!
+…pathetic…
+…come on… show me more…
+…making that face… in front of a goddess…
+…ahaha… pathetic pig…
+…that face… absolutely… disgraceful…
+…come on… crawl on the ground…
+…aha… the wind is laughing…
+…you think… you could look at a goddess…?
+…raise your head again… and you’re minced…
+…ahah… miserable mortal…
+…you’re… so easy to read…
+…ahaha… you’re hopeless…
+…pathetic… getting insulted… and enjoying it…
+…you… pervert…
+…ah… that just now… felt good, didn’t it…?
+…trash…
+…stay… worthless…
+…hey… do you have ulterior motives…?
+…ah… right on the mark…!
+…your mere existence… is irritating…aha…
+…truly… hopeless…pervert…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ehekatl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@3うみみゃあ！
+@3たらばがに！
+…スリ…
+…スリスリ…
+…ペロ…
+…ペロペロ…
+…コツン…
+…うみ…
+…みみみ…
+…み…</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">@3UMIMYAA!
+@3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">King crab!
+…rub…
+…rub rub…
+…lick…
+…lick lick…
+…bonk…
+…meo…
+…meo… w…
+…m… </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fox_maid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…おはようございます、ご主人さま…
+…お茶をお持ちしますね…
+…ご不在の間、お屋敷のことは私がきちんとお預かりしていました…
+…わ、私だけ…家族の中で胸が控えめなのは嫌です…
+…脚立…どこにありましたっけ…？
+…あ…お顔に、何かついてますよ…
+…ご主人さまの代わりに…私がやりますから…
+…あとどれくらい…お餅をつけばいいんでしょう…？
+…きゃあっ！…
+…ご、ご主人さま…！
+…お世話するのはメイドとしての務めですけど……たとえそうじゃなくても、私はします…
+…今夜のご夕食は…何になさいますか、ご主人さま…？
+…はい、あーん…♥
+…スッポンは…滋養にいいって聞きました…
+…高い棚のもの、抱き上げなくても大丈夫ですよ…？
+…ご主人さまとこんなに近いと…メイドとして、少し落ち着きません…
+…ちゃんと運動もしてくださいね…？
+…私…ちゃんとできてましたか、ご主人さま…？
+…ミ、ミルクですか…？ そ、それは……</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…Good morning, Master…
+…Allow me to serve you your tea…
+…I've stewarded your affairs while you were away…
+…I don't want to be the only flat one in my family…
+…Have you seen the stepladder…?
+…You have something on your face…
+…I'll gladly do it so you don't have to…
+…How much more mochi do I have to pound…?
+…Kyaaa!…
+…M-master…!
+…It's my duty to take care of you…but even if it weren't, I'd do it anyway…
+…What would you like for dinner tonight, Master…?
+…Open wide~♥
+…I've heard soft-shelled turtle is good for stamina…
+…You don't have to lift me so I can reach the high shelf…
+…It feels awkward to be this close with you when I'm your maid…
+…Be sure to get some exercise, okay…?
+…Did I do a good job, Master…?
+…Milk? B-but…</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -3446,96 +3629,172 @@
 米西利亚的魔女面包师，真是太厉害了！既是魔女，又是面包师！</t>
   </si>
   <si>
-    <t xml:space="preserve">@2…哔—…
-@2…沙沙沙…
-@2…沙沙…噶噶…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…抚摸…抚摸…
-@2…抱抱…
-@2…紧抱…
-@2…乖…乖…
-@2…笨…笨蛋…
-@2…别…别误会了…
-@2…才…才不是…为了你呢…
-@2…才…才不是…
-@2…只…只是想打发无聊的时间罢了…
-@2…嗯…那里…
-@2…嗯…请放松吧…
-@2…呼…呼—…
-@2…摸摸…摸摸…
-@2…迷茫的…人们啊…
-@2…治…治愈…
-@2…受伤的…灵魂…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…嘎吱…嘎吱嘎吱…
-@2…轰轰轰轰……
-@2…咯吱咯吱……
-@2…垮拉……
-@2…轰隆…哗啦……
-@2…咔哩…咔哩咔哩……
-@2…轰……轰—……
-@2…咯吱…咯吱吱吱……
-@2…咔吧……嘎吧吧……
-@2…喳啦……喳啦喳啦……
-@2…咚……咚……
-@2…咣……咣……
-@2…咚……
-@2…呼哈哈哈哈哈哈哈……
-@2…呼哈哈……呼哈啊……
-@2…呼哈哇……
-@2…呼……呼哈……
+    <t xml:space="preserve">我的料理中使用的都是顶级食材。
+想不想看看我的扫把收藏？
+嗯嗯…蝾螈的舌头…蜜蜂的眼睛。啊嗯？ 抱歉，没注意到你在这里。我正在思考新的食谱呢。
+咦，你有看到这附近有只猫吗？
+面包当然要用窑做呀？
+药品柜？  你给我好好看看，这是香料柜！
+我的帽子？　呵呵，很漂亮吧？
+（魔女把装满一袋的虫子哗啦一声都倒进了搅拌盆里。）
+……你的问题真多啊…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…哔—…
+…沙沙沙…
+…沙沙…嘎嘎…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…抚摸…抚摸…
+…抱抱…
+…紧抱…
+…乖…乖…
+…笨…笨蛋…
+…别…别误会了…
+…才…才不是…为了你呢…
+…才…才不是…
+…只…只是想打发无聊的时间罢了…
+…嗯…嘿咻…
+…被治愈吧…
+…呼…
+…咳…咳…
+…迷茫的…人们啊…
+…治…治愈…
+…受伤的…灵魂…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…嘎吱…嘎吱嘎吱…
+…轰轰轰轰……
+…咯吱咯吱……
+…垮拉……
+…轰隆…哗啦……
+…咔哩…咔哩咔哩……
+…轰……轰—……
+…咯吱…咯吱吱吱……
+…咔吧……嘎吧吧……
+…喳啦……喳啦喳啦……
+…咚……咚……
+…咣……咣……
+…咚……
+…呼哈哈哈哈哈哈哈……
+…呼哈哈……呼哈啊……
+…呼哈—……
+…呼……呼哈……
 @3呼哈哈哈哈哈哈哈！ 
-@3呼哈哇
-@2…呼呼……
-@2…呼—…！ …呼—…！……</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…别怕…妈妈会一直在你身边…
-@2…晚安…好孩子…
-@2…可以来…妈妈怀里哦…
-@2…只是好好活着…就很了不起了…
-@2…来…让我摸摸头…放心吧…
-@2…来…放松下来…
-@2…乖乖…
-@2…就这样…暖暖和和地…
-@2…摸摸…摸摸…力气，放松…
-@2…嗯…乖乖…好孩子…
-@2…就这样…暖暖的…
-@2…什么都…不用想了…
-@2…毛茸茸的…很安心吧…
-@2…用这尾巴…把你卷起来…
-@2…松松…软软…来…尾巴…
-@2…轻轻地…轻轻地…温柔…卷起…
-@2…温暖…温暖…你困了…
-@2…就这样…紧贴在一起…
-@2…吸…哈啊…一起…呼吸…
-@2…妈妈在哦…
-@2…摸摸…摸摸…力气，放松…
-@2…来…*紧紧抱住*…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@2…呵呵呵……
-@2…呵呵……
-@2…呵……呵呵呵……
-@2…呵呵……呵呵…
-@2…来吧……回去……
-@2…回到元素之中……
-@2…回去……
-@2…回到元素之中……呵呵……
-@2…呵……呵……呵……
-@2…呵……呵……
-@2…呵呵……呵……
-@2…快点……
-@2…呵呵呵呵……
-@2…呵呵呵呵呵……
-@2…呵呵……呵呵……呵呵……
-@2………
-@2………
-@2……奇异果……呵呵……
-@2……
-@2… </t>
+@3呼哈—
+…呼呼……
+…呼—…！ …呼—…！……</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…别怕…妈妈会一直在你身边…
+…晚安…好孩子…
+…可以来…妈妈怀里哦…
+…只是好好活着…就很了不起了…
+…来…让我摸摸头…放心吧…
+…来…放松下来…
+…乖乖…
+…就这样…暖暖和和地…
+…摸摸…摸摸…力气，放松…
+…嗯…乖乖…好孩子…
+…就这样…暖暖的…
+…什么都…不用想了…
+…毛茸茸的…很安心吧…
+…用这尾巴…把你卷起来…
+…松松…软软…来…尾巴…
+…轻轻地…轻轻地…温柔…卷起…
+…温暖…温暖…你困了…
+…就这样…紧贴在一起…
+…吸…哈啊…一起…呼吸…
+…妈妈在哦…
+…摸摸…摸摸…力气，放松…
+…来…*紧紧抱住*…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…呵呵呵……
+…呵呵……
+…呵……呵呵呵……
+…呵呵……呵呵…
+…回去吧……
+…回到元素之中……
+…回归……
+…向元素之中……呵呵……
+…呵……呵……呵……
+…呵……呵……
+…呵呵……呵……
+…快……
+…呵呵呵呵……
+…呵呵呵呵呵……
+…呵呵……呵呵……呵呵……
+………
+………
+……猕猴桃……呵呵……
+……
+… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">…哼…你喜欢这种的…？
+…真是个变态…
+…你这…蠢猪……啊哈哈……！
+…哎呀…在发抖呢……真可怜…
+…你喜欢…被看不起的感觉吧…？
+…区区蝼蚁……啊哈哈哈…
+…好小……真的……好小……
+…啊哈……真可笑……
+…啊哈哈……杂碎……真是杂碎……！
+…真可悲……
+…来…露出更多丑态吧…
+…在女神面前…真亏你能做出那种表情…
+…啊哈哈…可悲的猪猡…
+…那表情…真是…丢人至极…
+…快…给我趴在地上吧…
+…啊哈…连风都在嘲笑你…
+…谁允许你…直视女神了……？
+…再敢抬头的话…就把你剁成肉酱…
+…啊哈…可悲的凡人啊…
+…真是…好懂呢…
+…啊哈哈…没救的家伙…
+…丢人的家伙…挨了骂…还乐在其中…
+…这个…变态…
+…啊啊…刚才的…很让你开心吧…？
+…垃圾…
+…你就这样…毫无价值地存在下去吧…
+…你…该不会另有所图吧…？
+…啊啊…猜中了……啊哈哈！
+…光是存在就让人觉得…不舒服呢…啊哈…
+…真的是…无药可救的变态啊……</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@3喵咪咪！
+@3帝王蟹！
+…蹭…
+…蹭蹭…
+…舔…
+…舔舔…
+…咚…
+…喵咪…
+…咪咪咪…
+…咪…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…早上好，主人…
+…这就为您奉上茶水…
+…您不在的时候，宅邸的事务我都管理好了…
+…家族中只有我的胸部这么小…不甘心…
+…梯子…放到哪里去了…？
+…啊…您脸上沾上东西了哦…
+…请让我代替主人…来处理吧…
+…我还要捣…多久年糕呢…？
+…呀啊！…
+…主、主人…！
+…照顾您是女仆的职责……但就算不是职责，我也会做的…
+…今天的晚餐…想吃点什么呢，主人…？
+…来，张…嘴…♥
+…我听说甲鱼…十分的滋补…
+…架子高处的东西，不用抱起我也可以拿得到哦…？
+…和主人靠得这么近…作为女仆，有点静不下心…
+…记得适当运动哦…？
+…我…做的好吗，主人…？
+…奶…奶吗…？ 但、但是……</t>
   </si>
 </sst>
 </file>
@@ -3790,9 +4049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>280800</xdr:colOff>
+      <xdr:colOff>278280</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3802,7 +4061,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="49660200" cy="119520"/>
+          <a:ext cx="49657680" cy="117000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3980,7 +4239,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -3994,7 +4253,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -4008,7 +4267,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -4022,7 +4281,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -4036,7 +4295,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -4050,7 +4309,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -4064,7 +4323,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
@@ -4078,7 +4337,7 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
@@ -4092,7 +4351,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>29</v>
@@ -4106,7 +4365,7 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>32</v>
@@ -4120,7 +4379,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>35</v>
@@ -4134,7 +4393,7 @@
         <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
@@ -4148,7 +4407,7 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>41</v>
@@ -4162,7 +4421,7 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>44</v>
@@ -4176,7 +4435,7 @@
         <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>47</v>
@@ -4190,7 +4449,7 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>50</v>
@@ -4204,7 +4463,7 @@
         <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>53</v>
@@ -4218,7 +4477,7 @@
         <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>56</v>
@@ -4232,7 +4491,7 @@
         <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>59</v>
@@ -4246,7 +4505,7 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>62</v>
@@ -4260,7 +4519,7 @@
         <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>65</v>
@@ -4274,7 +4533,7 @@
         <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>68</v>
@@ -4288,7 +4547,7 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>71</v>
@@ -4302,7 +4561,7 @@
         <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>74</v>
@@ -4316,7 +4575,7 @@
         <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>77</v>
@@ -4330,7 +4589,7 @@
         <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>80</v>
@@ -4344,7 +4603,7 @@
         <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>83</v>
@@ -4358,7 +4617,7 @@
         <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>86</v>
@@ -4372,7 +4631,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>89</v>
@@ -4386,7 +4645,7 @@
         <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>92</v>
@@ -4400,7 +4659,7 @@
         <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>77</v>
@@ -4414,7 +4673,7 @@
         <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>80</v>
@@ -4428,7 +4687,7 @@
         <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>97</v>
@@ -4442,7 +4701,7 @@
         <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>100</v>
@@ -4456,7 +4715,7 @@
         <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>103</v>
@@ -4470,7 +4729,7 @@
         <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>106</v>
@@ -4484,7 +4743,7 @@
         <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>109</v>
@@ -4498,7 +4757,7 @@
         <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>112</v>
@@ -4512,7 +4771,7 @@
         <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>115</v>
@@ -4526,7 +4785,7 @@
         <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>118</v>
@@ -4540,7 +4799,7 @@
         <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>121</v>
@@ -4554,7 +4813,7 @@
         <v>123</v>
       </c>
       <c r="B46" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>124</v>
@@ -4568,7 +4827,7 @@
         <v>126</v>
       </c>
       <c r="B47" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>127</v>
@@ -4582,7 +4841,7 @@
         <v>129</v>
       </c>
       <c r="B48" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>130</v>
@@ -4596,7 +4855,7 @@
         <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>133</v>
@@ -4610,7 +4869,7 @@
         <v>135</v>
       </c>
       <c r="B50" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>136</v>
@@ -4624,7 +4883,7 @@
         <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>139</v>
@@ -4638,7 +4897,7 @@
         <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>142</v>
@@ -4652,7 +4911,7 @@
         <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>145</v>
@@ -4666,7 +4925,7 @@
         <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>148</v>
@@ -4680,7 +4939,7 @@
         <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>151</v>
@@ -4694,7 +4953,7 @@
         <v>153</v>
       </c>
       <c r="B56" t="s">
-        <v>524</v>
+        <v>536</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>154</v>
@@ -4708,7 +4967,7 @@
         <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>157</v>
@@ -4722,7 +4981,7 @@
         <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>160</v>
@@ -4736,7 +4995,7 @@
         <v>162</v>
       </c>
       <c r="B59" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>163</v>
@@ -4750,7 +5009,7 @@
         <v>165</v>
       </c>
       <c r="B60" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>166</v>
@@ -4764,7 +5023,7 @@
         <v>168</v>
       </c>
       <c r="B61" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>169</v>
@@ -4778,7 +5037,7 @@
         <v>171</v>
       </c>
       <c r="B62" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>172</v>
@@ -4792,7 +5051,7 @@
         <v>174</v>
       </c>
       <c r="B63" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>175</v>
@@ -4806,7 +5065,7 @@
         <v>177</v>
       </c>
       <c r="B64" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>178</v>
@@ -4820,7 +5079,7 @@
         <v>180</v>
       </c>
       <c r="B65" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>181</v>
@@ -4834,7 +5093,7 @@
         <v>183</v>
       </c>
       <c r="B66" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>184</v>
@@ -4848,7 +5107,7 @@
         <v>186</v>
       </c>
       <c r="B67" t="s">
-        <v>535</v>
+        <v>547</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>187</v>
@@ -4862,7 +5121,7 @@
         <v>189</v>
       </c>
       <c r="B68" t="s">
-        <v>536</v>
+        <v>548</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>190</v>
@@ -4876,7 +5135,7 @@
         <v>192</v>
       </c>
       <c r="B69" t="s">
-        <v>537</v>
+        <v>549</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>193</v>
@@ -4890,7 +5149,7 @@
         <v>195</v>
       </c>
       <c r="B70" t="s">
-        <v>538</v>
+        <v>550</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>196</v>
@@ -4904,7 +5163,7 @@
         <v>198</v>
       </c>
       <c r="B71" t="s">
-        <v>539</v>
+        <v>551</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>199</v>
@@ -4918,7 +5177,7 @@
         <v>201</v>
       </c>
       <c r="B72" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>202</v>
@@ -4932,7 +5191,7 @@
         <v>204</v>
       </c>
       <c r="B73" t="s">
-        <v>541</v>
+        <v>553</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>205</v>
@@ -4946,7 +5205,7 @@
         <v>207</v>
       </c>
       <c r="B74" t="s">
-        <v>542</v>
+        <v>554</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>208</v>
@@ -4960,7 +5219,7 @@
         <v>210</v>
       </c>
       <c r="B75" t="s">
-        <v>543</v>
+        <v>555</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>211</v>
@@ -4974,7 +5233,7 @@
         <v>213</v>
       </c>
       <c r="B76" t="s">
-        <v>544</v>
+        <v>556</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>214</v>
@@ -4988,7 +5247,7 @@
         <v>216</v>
       </c>
       <c r="B77" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>217</v>
@@ -5002,7 +5261,7 @@
         <v>219</v>
       </c>
       <c r="B78" t="s">
-        <v>546</v>
+        <v>558</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>220</v>
@@ -5016,7 +5275,7 @@
         <v>222</v>
       </c>
       <c r="B79" t="s">
-        <v>547</v>
+        <v>559</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>223</v>
@@ -5030,7 +5289,7 @@
         <v>225</v>
       </c>
       <c r="B80" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>226</v>
@@ -5044,7 +5303,7 @@
         <v>228</v>
       </c>
       <c r="B81" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>229</v>
@@ -5058,7 +5317,7 @@
         <v>231</v>
       </c>
       <c r="B82" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>232</v>
@@ -5087,11 +5346,11 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B23" sqref="B23"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8"/>
@@ -5130,7 +5389,7 @@
         <v>234</v>
       </c>
       <c r="B5" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>235</v>
@@ -5144,7 +5403,7 @@
         <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>552</v>
+        <v>564</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>238</v>
@@ -5158,7 +5417,7 @@
         <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>553</v>
+        <v>565</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>241</v>
@@ -5172,7 +5431,7 @@
         <v>243</v>
       </c>
       <c r="B8" t="s">
-        <v>554</v>
+        <v>566</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>244</v>
@@ -5186,7 +5445,7 @@
         <v>246</v>
       </c>
       <c r="B9" t="s">
-        <v>555</v>
+        <v>567</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>247</v>
@@ -5200,7 +5459,7 @@
         <v>249</v>
       </c>
       <c r="B10" t="s">
-        <v>556</v>
+        <v>568</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>250</v>
@@ -5214,7 +5473,7 @@
         <v>252</v>
       </c>
       <c r="B11" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>253</v>
@@ -5228,7 +5487,7 @@
         <v>255</v>
       </c>
       <c r="B12" t="s">
-        <v>558</v>
+        <v>570</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>256</v>
@@ -5242,7 +5501,7 @@
         <v>258</v>
       </c>
       <c r="B13" t="s">
-        <v>559</v>
+        <v>571</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>259</v>
@@ -5256,7 +5515,7 @@
         <v>261</v>
       </c>
       <c r="B14" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>262</v>
@@ -5270,7 +5529,7 @@
         <v>264</v>
       </c>
       <c r="B15" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>265</v>
@@ -5284,7 +5543,7 @@
         <v>267</v>
       </c>
       <c r="B16" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>268</v>
@@ -5298,7 +5557,7 @@
         <v>270</v>
       </c>
       <c r="B17" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>271</v>
@@ -5312,7 +5571,7 @@
         <v>273</v>
       </c>
       <c r="B18" t="s">
-        <v>564</v>
+        <v>576</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>274</v>
@@ -5326,7 +5585,7 @@
         <v>276</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>277</v>
@@ -5341,7 +5600,7 @@
         <v>279</v>
       </c>
       <c r="B20" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>280</v>
@@ -5355,7 +5614,7 @@
         <v>282</v>
       </c>
       <c r="B21" t="s">
-        <v>567</v>
+        <v>579</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>283</v>
@@ -5369,7 +5628,7 @@
         <v>285</v>
       </c>
       <c r="B22" t="s">
-        <v>568</v>
+        <v>580</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>286</v>
@@ -5383,7 +5642,7 @@
         <v>288</v>
       </c>
       <c r="B23" t="s">
-        <v>569</v>
+        <v>581</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>289</v>
@@ -5445,7 +5704,7 @@
         <v>291</v>
       </c>
       <c r="B5" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>292</v>
@@ -5459,7 +5718,7 @@
         <v>294</v>
       </c>
       <c r="B6" t="s">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>295</v>
@@ -5473,7 +5732,7 @@
         <v>297</v>
       </c>
       <c r="B7" t="s">
-        <v>572</v>
+        <v>584</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>298</v>
@@ -5487,7 +5746,7 @@
         <v>300</v>
       </c>
       <c r="B8" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>301</v>
@@ -5501,7 +5760,7 @@
         <v>303</v>
       </c>
       <c r="B9" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>304</v>
@@ -5515,7 +5774,7 @@
         <v>306</v>
       </c>
       <c r="B10" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>307</v>
@@ -5529,7 +5788,7 @@
         <v>309</v>
       </c>
       <c r="B11" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>310</v>
@@ -5543,7 +5802,7 @@
         <v>312</v>
       </c>
       <c r="B12" t="s">
-        <v>577</v>
+        <v>589</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>313</v>
@@ -5557,7 +5816,7 @@
         <v>315</v>
       </c>
       <c r="B13" t="s">
-        <v>578</v>
+        <v>590</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>316</v>
@@ -5571,7 +5830,7 @@
         <v>318</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>579</v>
+        <v>591</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>319</v>
@@ -5585,7 +5844,7 @@
         <v>321</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>322</v>
@@ -5599,7 +5858,7 @@
         <v>324</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>581</v>
+        <v>593</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>325</v>
@@ -5613,7 +5872,7 @@
         <v>327</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>328</v>
@@ -5638,14 +5897,14 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B47" sqref="B47"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B48" sqref="B48"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8"/>
@@ -5653,7 +5912,7 @@
     <col min="1" max="1" width="14.58" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.56" style="1" customWidth="1"/>
     <col min="3" max="3" width="110.96" style="1" customWidth="1"/>
-    <col min="4" max="4" width="100.58" style="1" customWidth="1"/>
+    <col min="4" max="4" width="139.81" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.8">
@@ -5679,12 +5938,12 @@
     <row r="4" ht="12.8">
       <c r="C4" s="3"/>
     </row>
-    <row r="5" ht="137.3">
+    <row r="5" ht="126.85">
       <c r="A5" s="1" t="s">
         <v>330</v>
       </c>
       <c r="B5" t="s">
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>331</v>
@@ -5698,7 +5957,7 @@
         <v>333</v>
       </c>
       <c r="B6" t="s">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>334</v>
@@ -5712,7 +5971,7 @@
         <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>337</v>
@@ -5726,7 +5985,7 @@
         <v>339</v>
       </c>
       <c r="B8" t="s">
-        <v>586</v>
+        <v>598</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>340</v>
@@ -5735,12 +5994,12 @@
         <v>341</v>
       </c>
     </row>
-    <row r="9" ht="116.4">
+    <row r="9" ht="105.95">
       <c r="A9" s="1" t="s">
         <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>587</v>
+        <v>599</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>343</v>
@@ -5749,12 +6008,12 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" ht="137.3">
+    <row r="10" ht="116.4">
       <c r="A10" s="1" t="s">
         <v>345</v>
       </c>
       <c r="B10" t="s">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>346</v>
@@ -5768,7 +6027,7 @@
         <v>348</v>
       </c>
       <c r="B11" t="s">
-        <v>589</v>
+        <v>601</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>349</v>
@@ -5782,7 +6041,7 @@
         <v>351</v>
       </c>
       <c r="B12" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>352</v>
@@ -5796,7 +6055,7 @@
         <v>354</v>
       </c>
       <c r="B13" t="s">
-        <v>591</v>
+        <v>603</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>355</v>
@@ -5810,7 +6069,7 @@
         <v>357</v>
       </c>
       <c r="B14" t="s">
-        <v>592</v>
+        <v>604</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>358</v>
@@ -5824,7 +6083,7 @@
         <v>360</v>
       </c>
       <c r="B15" t="s">
-        <v>593</v>
+        <v>605</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>361</v>
@@ -5838,7 +6097,7 @@
         <v>363</v>
       </c>
       <c r="B16" t="s">
-        <v>594</v>
+        <v>606</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>364</v>
@@ -5847,12 +6106,12 @@
         <v>365</v>
       </c>
     </row>
-    <row r="17" ht="53.7">
+    <row r="17" ht="43.25">
       <c r="A17" s="1" t="s">
         <v>366</v>
       </c>
       <c r="B17" t="s">
-        <v>595</v>
+        <v>607</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>367</v>
@@ -5861,12 +6120,12 @@
         <v>368</v>
       </c>
     </row>
-    <row r="18" ht="64.15">
+    <row r="18" ht="53.7">
       <c r="A18" s="1" t="s">
         <v>369</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>596</v>
+        <v>608</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>370</v>
@@ -5880,7 +6139,7 @@
         <v>372</v>
       </c>
       <c r="B19" t="s">
-        <v>597</v>
+        <v>609</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>373</v>
@@ -5894,7 +6153,7 @@
         <v>375</v>
       </c>
       <c r="B20" t="s">
-        <v>598</v>
+        <v>610</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>376</v>
@@ -5908,7 +6167,7 @@
         <v>378</v>
       </c>
       <c r="B21" t="s">
-        <v>599</v>
+        <v>611</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>379</v>
@@ -5922,7 +6181,7 @@
         <v>381</v>
       </c>
       <c r="B22" t="s">
-        <v>600</v>
+        <v>612</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>382</v>
@@ -5936,7 +6195,7 @@
         <v>384</v>
       </c>
       <c r="B23" t="s">
-        <v>601</v>
+        <v>613</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>385</v>
@@ -5950,7 +6209,7 @@
         <v>387</v>
       </c>
       <c r="B24" t="s">
-        <v>602</v>
+        <v>614</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>388</v>
@@ -5964,7 +6223,7 @@
         <v>390</v>
       </c>
       <c r="B25" t="s">
-        <v>603</v>
+        <v>615</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>391</v>
@@ -5978,7 +6237,7 @@
         <v>393</v>
       </c>
       <c r="B26" t="s">
-        <v>604</v>
+        <v>616</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>394</v>
@@ -5987,12 +6246,12 @@
         <v>395</v>
       </c>
     </row>
-    <row r="27" ht="91">
+    <row r="27" ht="79.1">
       <c r="A27" s="1" t="s">
         <v>396</v>
       </c>
       <c r="B27" t="s">
-        <v>605</v>
+        <v>617</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>397</v>
@@ -6001,12 +6260,12 @@
         <v>398</v>
       </c>
     </row>
-    <row r="28" ht="55.95">
+    <row r="28" ht="44.75">
       <c r="A28" s="1" t="s">
         <v>399</v>
       </c>
       <c r="B28" t="s">
-        <v>606</v>
+        <v>618</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>400</v>
@@ -6020,7 +6279,7 @@
         <v>402</v>
       </c>
       <c r="B29" t="s">
-        <v>607</v>
+        <v>619</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>403</v>
@@ -6034,7 +6293,7 @@
         <v>405</v>
       </c>
       <c r="B30" t="s">
-        <v>608</v>
+        <v>620</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>406</v>
@@ -6048,7 +6307,7 @@
         <v>408</v>
       </c>
       <c r="B31" t="s">
-        <v>609</v>
+        <v>621</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>409</v>
@@ -6062,7 +6321,7 @@
         <v>410</v>
       </c>
       <c r="B32" t="s">
-        <v>610</v>
+        <v>622</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>411</v>
@@ -6071,12 +6330,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="33" ht="95.5">
+    <row r="33" ht="91">
       <c r="A33" s="9" t="s">
         <v>413</v>
       </c>
       <c r="B33" t="s">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>414</v>
@@ -6090,7 +6349,7 @@
         <v>416</v>
       </c>
       <c r="B34" t="s">
-        <v>612</v>
+        <v>624</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>417</v>
@@ -6099,12 +6358,12 @@
         <v>418</v>
       </c>
     </row>
-    <row r="35" ht="126.85">
+    <row r="35" ht="105.95">
       <c r="A35" s="3" t="s">
         <v>419</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>613</v>
+        <v>625</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>420</v>
@@ -6118,7 +6377,7 @@
         <v>422</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>614</v>
+        <v>626</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>423</v>
@@ -6132,7 +6391,7 @@
         <v>425</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>615</v>
+        <v>627</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>426</v>
@@ -6146,7 +6405,7 @@
         <v>428</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>616</v>
+        <v>628</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>429</v>
@@ -6155,12 +6414,12 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" ht="85.05">
+    <row r="39" ht="74.6">
       <c r="A39" s="3" t="s">
         <v>431</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>617</v>
+        <v>629</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>432</v>
@@ -6174,7 +6433,7 @@
         <v>434</v>
       </c>
       <c r="B40" t="s">
-        <v>618</v>
+        <v>630</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>435</v>
@@ -6188,7 +6447,7 @@
         <v>437</v>
       </c>
       <c r="B41" t="s">
-        <v>619</v>
+        <v>631</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>438</v>
@@ -6202,7 +6461,7 @@
         <v>440</v>
       </c>
       <c r="B42" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>441</v>
@@ -6211,12 +6470,12 @@
         <v>442</v>
       </c>
     </row>
-    <row r="43" ht="116.4">
+    <row r="43" ht="105.95">
       <c r="A43" s="9" t="s">
         <v>443</v>
       </c>
       <c r="B43" t="s">
-        <v>621</v>
+        <v>633</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>444</v>
@@ -6225,12 +6484,12 @@
         <v>445</v>
       </c>
     </row>
-    <row r="44" ht="105.95">
+    <row r="44" ht="95.5">
       <c r="A44" s="9" t="s">
         <v>446</v>
       </c>
       <c r="B44" t="s">
-        <v>622</v>
+        <v>634</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>447</v>
@@ -6239,12 +6498,12 @@
         <v>448</v>
       </c>
     </row>
-    <row r="45" ht="158.2">
+    <row r="45" ht="116.4">
       <c r="A45" s="9" t="s">
         <v>449</v>
       </c>
       <c r="B45" t="s">
-        <v>623</v>
+        <v>635</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>450</v>
@@ -6253,12 +6512,12 @@
         <v>451</v>
       </c>
     </row>
-    <row r="46" ht="126.85">
+    <row r="46" ht="105.95">
       <c r="A46" s="9" t="s">
         <v>452</v>
       </c>
       <c r="B46" t="s">
-        <v>624</v>
+        <v>636</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>453</v>
@@ -6272,13 +6531,27 @@
         <v>455</v>
       </c>
       <c r="B47" t="s">
-        <v>625</v>
+        <v>637</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>456</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>457</v>
+      </c>
+    </row>
+    <row r="48" ht="95.5">
+      <c r="A48" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B48" t="s">
+        <v>638</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -6297,14 +6570,14 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B9" sqref="B9"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B12" sqref="B12"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8"/>
@@ -6340,72 +6613,114 @@
     </row>
     <row r="5" ht="32.8">
       <c r="A5" s="1" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B5" t="s">
-        <v>626</v>
+        <v>639</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" ht="168.65">
       <c r="A6" s="1" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B6" t="s">
-        <v>627</v>
+        <v>640</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" ht="220.85">
       <c r="A7" s="1" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B7" t="s">
-        <v>628</v>
+        <v>641</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" ht="231.3">
       <c r="A8" s="1" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B8" t="s">
-        <v>629</v>
+        <v>642</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" ht="210.4">
       <c r="A9" s="1" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="B9" t="s">
-        <v>630</v>
+        <v>643</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>472</v>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="10" ht="314.9">
+      <c r="A10" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B10" t="s">
+        <v>644</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="11" ht="112.65">
+      <c r="A11" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B11" t="s">
+        <v>645</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" ht="199.95">
+      <c r="A12" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B12" t="s">
+        <v>646</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>